<commit_message>
rename NewReferences sheet to 'New references'
</commit_message>
<xml_diff>
--- a/tests/fixtures/data_file_2.xlsx
+++ b/tests/fixtures/data_file_2.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19800" yWindow="3700" windowWidth="17540" windowHeight="9540" activeTab="1"/>
+    <workbookView xWindow="-19000" yWindow="880" windowWidth="13340" windowHeight="9540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Git metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Tests" sheetId="2" r:id="rId2"/>
-    <sheet name="NewReferences" sheetId="3" r:id="rId3"/>
+    <sheet name="New references" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewReferences!$A$1:$B$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'New references'!$A$1:$B$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="124519" concurrentCalc="0"/>
@@ -667,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>